<commit_message>
Documentacion adicional y cambios que faltaban
</commit_message>
<xml_diff>
--- a/Documentacion/drafts/20120521/Tests de velocidad del nodo mas simple.xlsx
+++ b/Documentacion/drafts/20120521/Tests de velocidad del nodo mas simple.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28635" windowHeight="12780"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="28635" windowHeight="12780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="26-05-2012" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>X1</t>
   </si>
@@ -61,6 +61,48 @@
   </si>
   <si>
     <t>Milis por mensaje</t>
+  </si>
+  <si>
+    <t>[1/0ms -&gt;(1)-&gt;10]</t>
+  </si>
+  <si>
+    <t>[1/0ms -&gt;(1)-&gt;1]</t>
+  </si>
+  <si>
+    <t>[10/1ms -&gt;(1)-&gt;10]</t>
+  </si>
+  <si>
+    <t>[1/0ms -&gt;(10)-&gt;1]</t>
+  </si>
+  <si>
+    <t>Input(msg/ms)</t>
+  </si>
+  <si>
+    <t>TestMessagePerformance</t>
+  </si>
+  <si>
+    <t>Output(individual)</t>
+  </si>
+  <si>
+    <t>Output Total</t>
+  </si>
+  <si>
+    <t>OT/I</t>
+  </si>
+  <si>
+    <t>O(i)/I</t>
+  </si>
+  <si>
+    <t>[1/0ms -&gt;(10)S-&gt;1]</t>
+  </si>
+  <si>
+    <t>[10/1ms -&gt;(10)-&gt;1]</t>
+  </si>
+  <si>
+    <t>[10/1ms -&gt;(10)S-&gt;1]</t>
+  </si>
+  <si>
+    <t>TestMessagePerformance (con medición de delivery)</t>
   </si>
 </sst>
 </file>
@@ -68,7 +110,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -99,10 +141,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,11 +649,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="92333568"/>
-        <c:axId val="92335488"/>
+        <c:axId val="161972608"/>
+        <c:axId val="161974144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="92333568"/>
+        <c:axId val="161972608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,7 +662,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92335488"/>
+        <c:crossAx val="161974144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -627,7 +670,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92335488"/>
+        <c:axId val="161974144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -638,14 +681,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92333568"/>
+        <c:crossAx val="161972608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1149,11 +1191,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="167087488"/>
-        <c:axId val="167089280"/>
+        <c:axId val="162601216"/>
+        <c:axId val="162615296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="167087488"/>
+        <c:axId val="162601216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1162,7 +1204,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167089280"/>
+        <c:crossAx val="162615296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1170,7 +1212,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="167089280"/>
+        <c:axId val="162615296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1181,14 +1223,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="167087488"/>
+        <c:crossAx val="162601216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1557,7 +1598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -1888,13 +1929,440 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D4:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="3">
+        <v>41055</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2">
+        <v>40.019171130532797</v>
+      </c>
+      <c r="F6" s="2">
+        <v>6.5296494690348599</v>
+      </c>
+      <c r="G6" s="2">
+        <v>65.294239263227098</v>
+      </c>
+      <c r="H6">
+        <f>F6/E6</f>
+        <v>0.16316303622922954</v>
+      </c>
+      <c r="I6">
+        <f>G6/E6</f>
+        <v>1.6315740036257418</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2">
+        <v>196.59639999999999</v>
+      </c>
+      <c r="F7" s="2">
+        <v>196.5958</v>
+      </c>
+      <c r="G7" s="2">
+        <v>196.5958</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H9" si="0">F7/E7</f>
+        <v>0.99999694806212125</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I9" si="1">G7/E7</f>
+        <v>0.99999694806212125</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5.1208</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5.1201999999999996</v>
+      </c>
+      <c r="G8" s="2">
+        <v>51.201999999999998</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.99988283080768625</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>9.9988283080768632</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2">
+        <v>96.110245940556396</v>
+      </c>
+      <c r="F9" s="2">
+        <v>11.9188111290475</v>
+      </c>
+      <c r="G9" s="2">
+        <v>11.9188111290475</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.12401186795858593</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0.12401186795858593</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2">
+        <v>88.594641987335606</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2.1042377009254699E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2.1042377009254699E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ref="H10:H12" si="2">F10/E10</f>
+        <v>2.3751297524586936E-4</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ref="I10:I12" si="3">G10/E10</f>
+        <v>2.3751297524586936E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5.0744882675985998</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5.0740888666999497</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5.0740888666999497</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>0.99992129237913496</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>0.99992129237913496</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5.1210000000000004</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5.1201999999999996</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5.1201999999999996</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>0.99984378051161871</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>0.99984378051161871</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="3">
+        <v>41056</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2">
+        <v>37.970952380952298</v>
+      </c>
+      <c r="F18" s="2">
+        <v>9.2284761904761901</v>
+      </c>
+      <c r="G18" s="2">
+        <v>92.282476190476103</v>
+      </c>
+      <c r="H18">
+        <f>F18/E18</f>
+        <v>0.24304041936818924</v>
+      </c>
+      <c r="I18">
+        <f>G18/E18</f>
+        <v>2.4303439972911653</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="2">
+        <v>158.46</v>
+      </c>
+      <c r="F19" s="2">
+        <v>158.45840000000001</v>
+      </c>
+      <c r="G19" s="2">
+        <v>158.45840000000001</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ref="H19:H24" si="4">F19/E19</f>
+        <v>0.99998990281459044</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ref="I19:I24" si="5">G19/E19</f>
+        <v>0.99998990281459044</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5.1210000000000004</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5.1204000000000001</v>
+      </c>
+      <c r="G20" s="2">
+        <v>51.204000000000001</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="4"/>
+        <v>0.99988283538371403</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="5"/>
+        <v>9.9988283538371405</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="2">
+        <v>72.599047619047596</v>
+      </c>
+      <c r="F21" s="2">
+        <v>9.7200952380952295</v>
+      </c>
+      <c r="G21" s="2">
+        <v>9.7200952380952295</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>0.13388736570071749</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="5"/>
+        <v>0.13388736570071749</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="2">
+        <v>60.284599999999998</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.34770000000000001</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.34770000000000001</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="4"/>
+        <v>5.7676421507316961E-3</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="5"/>
+        <v>5.7676421507316961E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="2">
+        <v>5.0815999999999999</v>
+      </c>
+      <c r="F23" s="2">
+        <v>5.0815999999999999</v>
+      </c>
+      <c r="G23" s="2">
+        <v>5.0815999999999999</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5.1211000000000002</v>
+      </c>
+      <c r="F24" s="2">
+        <v>5.1205999999999996</v>
+      </c>
+      <c r="G24" s="2">
+        <v>5.1205999999999996</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="4"/>
+        <v>0.99990236472632821</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="5"/>
+        <v>0.99990236472632821</v>
+      </c>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H6:I12">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18:I24">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0.5"/>
+        <cfvo type="num" val="0.9"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <color theme="6" tint="0.59999389629810485"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>